<commit_message>
Update web whatsapp HLR And Test Case.xlsx
</commit_message>
<xml_diff>
--- a/Assignment/Module 2/web whatsapp HLR And Test Case.xlsx
+++ b/Assignment/Module 2/web whatsapp HLR And Test Case.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="HLR" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="28">
   <si>
     <t>Functionality Id</t>
   </si>
@@ -82,6 +82,36 @@
   </si>
   <si>
     <t>when we scan the QR Code From the device Whatsapp open properly on desktop.</t>
+  </si>
+  <si>
+    <t>intenet and browser must be in the working condition</t>
+  </si>
+  <si>
+    <t>1) web.whatsapp.com 2) press enter key
+3) scan the QR code</t>
+  </si>
+  <si>
+    <t>1) web.whatsapp.com 2) press enter key</t>
+  </si>
+  <si>
+    <t>1) web.whatsapp.com 2) press enter key
+3) click on video play button</t>
+  </si>
+  <si>
+    <t>to open the website properly</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>as per expected result</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>1) web.whatsapp.com 2) press enter key
+3) click on need help to get started link</t>
   </si>
 </sst>
 </file>
@@ -139,13 +169,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -429,8 +468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,8 +543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,9 +553,10 @@
     <col min="2" max="2" width="19.42578125" customWidth="1"/>
     <col min="3" max="3" width="18.85546875" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="26" customWidth="1"/>
     <col min="6" max="6" width="16.28515625" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="56.25" x14ac:dyDescent="0.25">
@@ -548,53 +588,121 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="93.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="187.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="225" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="225" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="6" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>

</xml_diff>